<commit_message>
Gjort nya avstånd till närmsta föryngring med korrekt kullar och kullarna 2018. Uppdaterat relativt mått på kullar-skriptet så att filen med korrekt antal kullar läses in.
</commit_message>
<xml_diff>
--- a/Rawdata/distans närmsta förynging.xlsx
+++ b/Rawdata/distans närmsta förynging.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C172"/>
+  <dimension ref="A1:C186"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -377,76 +377,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2000-FSZZ019</t>
+          <t>2001-FSZZ020</t>
         </is>
       </c>
       <c r="B2">
-        <v>24386.59385810163</v>
+        <v>8667.09714956513</v>
       </c>
       <c r="C2">
-        <v>2000</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2000-FSZZ032</t>
+          <t>2001-FSZZ033</t>
         </is>
       </c>
       <c r="B3">
-        <v>24386.59385810163</v>
+        <v>8667.09714956513</v>
       </c>
       <c r="C3">
-        <v>2000</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>2001-FSZZ020</t>
+          <t>2002-FSZZ020</t>
         </is>
       </c>
       <c r="B4">
-        <v>8667.09714956513</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C4">
-        <v>2001</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>2001-FSZZ031</t>
+          <t>2002-FSZZ031</t>
         </is>
       </c>
       <c r="B5">
         <v>4295.235732762522</v>
       </c>
       <c r="C5">
-        <v>2001</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2001-FSZZ033</t>
+          <t>2002-FSZZ032</t>
         </is>
       </c>
       <c r="B6">
-        <v>4295.235732762522</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C6">
-        <v>2001</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2002-FSZZ020</t>
+          <t>2002-FSZZ033</t>
         </is>
       </c>
       <c r="B7">
-        <v>4974.737983049961</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C7">
         <v>2002</v>
@@ -455,50 +455,50 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2002-FSZZ031</t>
+          <t>2004-FSZZ020</t>
         </is>
       </c>
       <c r="B8">
-        <v>4295.235732762522</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C8">
-        <v>2002</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2002-FSZZ032</t>
+          <t>2004-FSZZ024</t>
         </is>
       </c>
       <c r="B9">
-        <v>4974.737983049961</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C9">
-        <v>2002</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2002-FSZZ033</t>
+          <t>2004-FSZZ031</t>
         </is>
       </c>
       <c r="B10">
         <v>4295.235732762522</v>
       </c>
       <c r="C10">
-        <v>2002</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2004-FSZZ020</t>
+          <t>2004-FSZZ033</t>
         </is>
       </c>
       <c r="B11">
-        <v>8152.76425514684</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C11">
         <v>2004</v>
@@ -507,50 +507,50 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>2004-FSZZ024</t>
+          <t>2005-FSZZ020</t>
         </is>
       </c>
       <c r="B12">
-        <v>8152.76425514684</v>
+        <v>6221.830679149023</v>
       </c>
       <c r="C12">
-        <v>2004</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2004-FSZZ031</t>
+          <t>2005-FSZZ024</t>
         </is>
       </c>
       <c r="B13">
-        <v>4295.235732762522</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C13">
-        <v>2004</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2004-FSZZ033</t>
+          <t>2005-FSZZ029</t>
         </is>
       </c>
       <c r="B14">
-        <v>4295.235732762522</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C14">
-        <v>2004</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>2005-FSZZ013</t>
+          <t>2005-FSZZ031</t>
         </is>
       </c>
       <c r="B15">
-        <v>13687.6198442242</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C15">
         <v>2005</v>
@@ -559,11 +559,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2005-FSZZ020</t>
+          <t>2005-FSZZ033</t>
         </is>
       </c>
       <c r="B16">
-        <v>6221.654120891003</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C16">
         <v>2005</v>
@@ -572,11 +572,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2005-FSZZ024</t>
+          <t>2005-FSZZ034</t>
         </is>
       </c>
       <c r="B17">
-        <v>8152.76425514684</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C17">
         <v>2005</v>
@@ -585,63 +585,63 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2005-FSZZ029</t>
+          <t>2007-FSZZ010</t>
         </is>
       </c>
       <c r="B18">
-        <v>4997.357801878909</v>
+        <v>17742.88589829738</v>
       </c>
       <c r="C18">
-        <v>2005</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2005-FSZZ031</t>
+          <t>2007-FSZZ014</t>
         </is>
       </c>
       <c r="B19">
-        <v>4295.235732762522</v>
+        <v>13502.29610103408</v>
       </c>
       <c r="C19">
-        <v>2005</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>2005-FSZZ033</t>
+          <t>2007-FSZZ018</t>
         </is>
       </c>
       <c r="B20">
-        <v>3188.160127722571</v>
+        <v>8043.570662336472</v>
       </c>
       <c r="C20">
-        <v>2005</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2005-FSZZ034</t>
+          <t>2007-FSZZ020</t>
         </is>
       </c>
       <c r="B21">
-        <v>3188.160127722571</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C21">
-        <v>2005</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>2007-FSZZ010</t>
+          <t>2007-FSZZ024</t>
         </is>
       </c>
       <c r="B22">
-        <v>17742.88589829738</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C22">
         <v>2007</v>
@@ -650,11 +650,11 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2007-FSZZ014</t>
+          <t>2007-FSZZ029</t>
         </is>
       </c>
       <c r="B23">
-        <v>13503.13448796242</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C23">
         <v>2007</v>
@@ -663,11 +663,11 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2007-FSZZ018</t>
+          <t>2007-FSZZ031</t>
         </is>
       </c>
       <c r="B24">
-        <v>3752.443603840036</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C24">
         <v>2007</v>
@@ -676,11 +676,11 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>2007-FSZZ020</t>
+          <t>2007-FSZZ033</t>
         </is>
       </c>
       <c r="B25">
-        <v>8152.76425514684</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C25">
         <v>2007</v>
@@ -689,11 +689,11 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2007-FSZZ024</t>
+          <t>2007-FSZZ042</t>
         </is>
       </c>
       <c r="B26">
-        <v>8152.76425514684</v>
+        <v>8043.570662336472</v>
       </c>
       <c r="C26">
         <v>2007</v>
@@ -702,76 +702,76 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2007-FSZZ029</t>
+          <t>2008-FSZZ010</t>
         </is>
       </c>
       <c r="B27">
-        <v>4997.357801878909</v>
+        <v>15291.63097906826</v>
       </c>
       <c r="C27">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>2007-FSZZ031</t>
+          <t>2008-FSZZ013</t>
         </is>
       </c>
       <c r="B28">
-        <v>4295.235732762522</v>
+        <v>2021.19222242715</v>
       </c>
       <c r="C28">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2007-FSZZ033</t>
+          <t>2008-FSZZ015</t>
         </is>
       </c>
       <c r="B29">
-        <v>4295.235732762522</v>
+        <v>4429.673238513197</v>
       </c>
       <c r="C29">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>2007-FSZZ042</t>
+          <t>2008-FSZZ018</t>
         </is>
       </c>
       <c r="B30">
-        <v>8043.570662336472</v>
+        <v>4429.673238513197</v>
       </c>
       <c r="C30">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>2007-FSZZ059</t>
+          <t>2008-FSZZ019</t>
         </is>
       </c>
       <c r="B31">
-        <v>3752.443603840036</v>
+        <v>5087.597664910228</v>
       </c>
       <c r="C31">
-        <v>2007</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2008-FSZZ010</t>
+          <t>2008-FSZZ020</t>
         </is>
       </c>
       <c r="B32">
-        <v>15291.63097906826</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C32">
         <v>2008</v>
@@ -780,11 +780,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2008-FSZZ013</t>
+          <t>2008-FSZZ024</t>
         </is>
       </c>
       <c r="B33">
-        <v>2021.19222242715</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C33">
         <v>2008</v>
@@ -793,11 +793,11 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2008-FSZZ015</t>
+          <t>2008-FSZZ029</t>
         </is>
       </c>
       <c r="B34">
-        <v>4429.673238513197</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C34">
         <v>2008</v>
@@ -806,11 +806,11 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2008-FSZZ018</t>
+          <t>2008-FSZZ031</t>
         </is>
       </c>
       <c r="B35">
-        <v>4429.673238513197</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C35">
         <v>2008</v>
@@ -819,11 +819,11 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2008-FSZZ019</t>
+          <t>2008-FSZZ032</t>
         </is>
       </c>
       <c r="B36">
-        <v>5087.597664910228</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C36">
         <v>2008</v>
@@ -832,11 +832,11 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2008-FSZZ020</t>
+          <t>2008-FSZZ033</t>
         </is>
       </c>
       <c r="B37">
-        <v>4974.737983049961</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C37">
         <v>2008</v>
@@ -845,11 +845,11 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>2008-FSZZ024</t>
+          <t>2008-FSZZ035</t>
         </is>
       </c>
       <c r="B38">
-        <v>8152.76425514684</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C38">
         <v>2008</v>
@@ -858,11 +858,11 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2008-FSZZ029</t>
+          <t>2008-FSZZ042</t>
         </is>
       </c>
       <c r="B39">
-        <v>4997.357801878909</v>
+        <v>8043.570662336472</v>
       </c>
       <c r="C39">
         <v>2008</v>
@@ -871,11 +871,11 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2008-FSZZ031</t>
+          <t>2008-FSZZ090</t>
         </is>
       </c>
       <c r="B40">
-        <v>1891.979915326799</v>
+        <v>2021.19222242715</v>
       </c>
       <c r="C40">
         <v>2008</v>
@@ -884,115 +884,115 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2008-FSZZ032</t>
+          <t>2009-FSZZ018</t>
         </is>
       </c>
       <c r="B41">
-        <v>4974.737983049961</v>
+        <v>11608.02429356521</v>
       </c>
       <c r="C41">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2008-FSZZ033</t>
+          <t>2009-FSZZ024</t>
         </is>
       </c>
       <c r="B42">
-        <v>4295.235732762522</v>
+        <v>11608.02429356521</v>
       </c>
       <c r="C42">
-        <v>2008</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>2008-FSZZ035</t>
+          <t>2010-FSZZ010</t>
         </is>
       </c>
       <c r="B43">
-        <v>1891.979915326799</v>
+        <v>15291.63097906826</v>
       </c>
       <c r="C43">
-        <v>2008</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>2008-FSZZ042</t>
+          <t>2010-FSZZ013</t>
         </is>
       </c>
       <c r="B44">
-        <v>8043.570662336472</v>
+        <v>6788.743992816344</v>
       </c>
       <c r="C44">
-        <v>2008</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2008-FSZZ080</t>
+          <t>2010-FSZZ014</t>
         </is>
       </c>
       <c r="B45">
-        <v>3314.697572931805</v>
+        <v>7564.3324226266</v>
       </c>
       <c r="C45">
-        <v>2008</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2008-FSZZ090</t>
+          <t>2010-FSZZ018</t>
         </is>
       </c>
       <c r="B46">
-        <v>2021.19222242715</v>
+        <v>6396.034474578761</v>
       </c>
       <c r="C46">
-        <v>2008</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>2009-FSZZ018</t>
+          <t>2010-FSZZ019</t>
         </is>
       </c>
       <c r="B47">
-        <v>11608.02429356521</v>
+        <v>6396.034474578761</v>
       </c>
       <c r="C47">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>2009-FSZZ024</t>
+          <t>2010-FSZZ020</t>
         </is>
       </c>
       <c r="B48">
-        <v>11608.02429356521</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C48">
-        <v>2009</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>2010-FSZZ010</t>
+          <t>2010-FSZZ024</t>
         </is>
       </c>
       <c r="B49">
-        <v>15291.63097906826</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C49">
         <v>2010</v>
@@ -1001,11 +1001,11 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>2010-FSZZ013</t>
+          <t>2010-FSZZ029</t>
         </is>
       </c>
       <c r="B50">
-        <v>5167.092993163564</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C50">
         <v>2010</v>
@@ -1014,11 +1014,11 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>2010-FSZZ014</t>
+          <t>2010-FSZZ031</t>
         </is>
       </c>
       <c r="B51">
-        <v>7564.951288673312</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C51">
         <v>2010</v>
@@ -1027,11 +1027,11 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>2010-FSZZ015</t>
+          <t>2010-FSZZ032</t>
         </is>
       </c>
       <c r="B52">
-        <v>4429.673238513197</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C52">
         <v>2010</v>
@@ -1040,11 +1040,11 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>2010-FSZZ018</t>
+          <t>2010-FSZZ033</t>
         </is>
       </c>
       <c r="B53">
-        <v>4429.673238513197</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C53">
         <v>2010</v>
@@ -1053,11 +1053,11 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>2010-FSZZ019</t>
+          <t>2010-FSZZ042</t>
         </is>
       </c>
       <c r="B54">
-        <v>5087.597664910228</v>
+        <v>8043.570662336472</v>
       </c>
       <c r="C54">
         <v>2010</v>
@@ -1066,11 +1066,11 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>2010-FSZZ020</t>
+          <t>2010-FSZZ064</t>
         </is>
       </c>
       <c r="B55">
-        <v>4974.737983049961</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C55">
         <v>2010</v>
@@ -1079,102 +1079,102 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>2010-FSZZ024</t>
+          <t>2011-FSZZ009</t>
         </is>
       </c>
       <c r="B56">
-        <v>8152.76425514684</v>
+        <v>3876.480878322503</v>
       </c>
       <c r="C56">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>2010-FSZZ027</t>
+          <t>2011-FSZZ010</t>
         </is>
       </c>
       <c r="B57">
-        <v>6969.405211350535</v>
+        <v>15291.63097906826</v>
       </c>
       <c r="C57">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>2010-FSZZ029</t>
+          <t>2011-FSZZ012</t>
         </is>
       </c>
       <c r="B58">
-        <v>4997.357801878909</v>
+        <v>3443.106736655139</v>
       </c>
       <c r="C58">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>2010-FSZZ031</t>
+          <t>2011-FSZZ013</t>
         </is>
       </c>
       <c r="B59">
-        <v>4295.235732762522</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C59">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>2010-FSZZ032</t>
+          <t>2011-FSZZ014</t>
         </is>
       </c>
       <c r="B60">
-        <v>4974.737983049961</v>
+        <v>7564.3324226266</v>
       </c>
       <c r="C60">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>2010-FSZZ033</t>
+          <t>2011-FSZZ015</t>
         </is>
       </c>
       <c r="B61">
-        <v>4295.235732762522</v>
+        <v>3476.736975958923</v>
       </c>
       <c r="C61">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>2010-FSZZ042</t>
+          <t>2011-FSZZ016</t>
         </is>
       </c>
       <c r="B62">
-        <v>6969.405211350535</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C62">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>2011-FSZZ009</t>
+          <t>2011-FSZZ018</t>
         </is>
       </c>
       <c r="B63">
-        <v>3876.480878322503</v>
+        <v>3999.901123777936</v>
       </c>
       <c r="C63">
         <v>2011</v>
@@ -1183,11 +1183,11 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>2011-FSZZ010</t>
+          <t>2011-FSZZ019</t>
         </is>
       </c>
       <c r="B64">
-        <v>16446.39161031988</v>
+        <v>5087.597664910228</v>
       </c>
       <c r="C64">
         <v>2011</v>
@@ -1196,11 +1196,11 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>2011-FSZZ012</t>
+          <t>2011-FSZZ020</t>
         </is>
       </c>
       <c r="B65">
-        <v>3443.106736655139</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C65">
         <v>2011</v>
@@ -1209,11 +1209,11 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>2011-FSZZ013</t>
+          <t>2011-FSZZ024</t>
         </is>
       </c>
       <c r="B66">
-        <v>2790.894121961634</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C66">
         <v>2011</v>
@@ -1222,11 +1222,11 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>2011-FSZZ014</t>
+          <t>2011-FSZZ027</t>
         </is>
       </c>
       <c r="B67">
-        <v>7564.951288673312</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C67">
         <v>2011</v>
@@ -1235,11 +1235,11 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>2011-FSZZ015</t>
+          <t>2011-FSZZ028</t>
         </is>
       </c>
       <c r="B68">
-        <v>3476.736975958923</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C68">
         <v>2011</v>
@@ -1248,11 +1248,11 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>2011-FSZZ016</t>
+          <t>2011-FSZZ029</t>
         </is>
       </c>
       <c r="B69">
-        <v>2790.894121961634</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C69">
         <v>2011</v>
@@ -1261,11 +1261,11 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>2011-FSZZ018</t>
+          <t>2011-FSZZ030</t>
         </is>
       </c>
       <c r="B70">
-        <v>3999.901123777936</v>
+        <v>3443.106736655139</v>
       </c>
       <c r="C70">
         <v>2011</v>
@@ -1274,11 +1274,11 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>2011-FSZZ019</t>
+          <t>2011-FSZZ031</t>
         </is>
       </c>
       <c r="B71">
-        <v>5087.597664910228</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C71">
         <v>2011</v>
@@ -1287,11 +1287,11 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>2011-FSZZ020</t>
+          <t>2011-FSZZ032</t>
         </is>
       </c>
       <c r="B72">
-        <v>7764.063691134946</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C72">
         <v>2011</v>
@@ -1300,11 +1300,11 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>2011-FSZZ024</t>
+          <t>2011-FSZZ033</t>
         </is>
       </c>
       <c r="B73">
-        <v>2194.10346155326</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C73">
         <v>2011</v>
@@ -1313,11 +1313,11 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>2011-FSZZ027</t>
+          <t>2011-FSZZ035</t>
         </is>
       </c>
       <c r="B74">
-        <v>2563.112365855231</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C74">
         <v>2011</v>
@@ -1326,11 +1326,11 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>2011-FSZZ028</t>
+          <t>2011-FSZZ036</t>
         </is>
       </c>
       <c r="B75">
-        <v>2563.112365855231</v>
+        <v>8413.182275453208</v>
       </c>
       <c r="C75">
         <v>2011</v>
@@ -1339,11 +1339,11 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>2011-FSZZ029</t>
+          <t>2011-FSZZ042</t>
         </is>
       </c>
       <c r="B76">
-        <v>4997.357801878909</v>
+        <v>6969.405211350535</v>
       </c>
       <c r="C76">
         <v>2011</v>
@@ -1352,11 +1352,11 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>2011-FSZZ030</t>
+          <t>2011-FSZZ064</t>
         </is>
       </c>
       <c r="B77">
-        <v>3443.106736655139</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C77">
         <v>2011</v>
@@ -1365,11 +1365,11 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>2011-FSZZ031</t>
+          <t>2011-FSZZ066</t>
         </is>
       </c>
       <c r="B78">
-        <v>1891.979915326799</v>
+        <v>4417.651978144046</v>
       </c>
       <c r="C78">
         <v>2011</v>
@@ -1378,11 +1378,11 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>2011-FSZZ033</t>
+          <t>2011-FSZZ080</t>
         </is>
       </c>
       <c r="B79">
-        <v>4295.235732762522</v>
+        <v>3314.697572931805</v>
       </c>
       <c r="C79">
         <v>2011</v>
@@ -1391,11 +1391,11 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>2011-FSZZ035</t>
+          <t>2011-FSZZ108</t>
         </is>
       </c>
       <c r="B80">
-        <v>1891.979915326799</v>
+        <v>22829.27946738574</v>
       </c>
       <c r="C80">
         <v>2011</v>
@@ -1404,76 +1404,76 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>2011-FSZZ036</t>
+          <t>2013-FSZZ009</t>
         </is>
       </c>
       <c r="B81">
-        <v>8413.182275453208</v>
+        <v>3876.480878322503</v>
       </c>
       <c r="C81">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>2011-FSZZ042</t>
+          <t>2013-FSZZ012</t>
         </is>
       </c>
       <c r="B82">
-        <v>6969.405211350535</v>
+        <v>3443.106736655139</v>
       </c>
       <c r="C82">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>2011-FSZZ064</t>
+          <t>2013-FSZZ013</t>
         </is>
       </c>
       <c r="B83">
-        <v>2194.10346155326</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C83">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>2011-FSZZ066</t>
+          <t>2013-FSZZ015</t>
         </is>
       </c>
       <c r="B84">
-        <v>4417.651978144046</v>
+        <v>3476.736975958923</v>
       </c>
       <c r="C84">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>2011-FSZZ080</t>
+          <t>2013-FSZZ016</t>
         </is>
       </c>
       <c r="B85">
-        <v>3314.697572931805</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C85">
-        <v>2011</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>2013-FSZZ009</t>
+          <t>2013-FSZZ020</t>
         </is>
       </c>
       <c r="B86">
-        <v>3876.480878322503</v>
+        <v>6221.830679149023</v>
       </c>
       <c r="C86">
         <v>2013</v>
@@ -1482,11 +1482,11 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>2013-FSZZ012</t>
+          <t>2013-FSZZ024</t>
         </is>
       </c>
       <c r="B87">
-        <v>3443.106736655139</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C87">
         <v>2013</v>
@@ -1495,11 +1495,11 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>2013-FSZZ013</t>
+          <t>2013-FSZZ027</t>
         </is>
       </c>
       <c r="B88">
-        <v>2790.894121961634</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C88">
         <v>2013</v>
@@ -1508,11 +1508,11 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>2013-FSZZ015</t>
+          <t>2013-FSZZ028</t>
         </is>
       </c>
       <c r="B89">
-        <v>3476.736975958923</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C89">
         <v>2013</v>
@@ -1521,11 +1521,11 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>2013-FSZZ016</t>
+          <t>2013-FSZZ029</t>
         </is>
       </c>
       <c r="B90">
-        <v>2790.894121961634</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C90">
         <v>2013</v>
@@ -1534,11 +1534,11 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>2013-FSZZ020</t>
+          <t>2013-FSZZ030</t>
         </is>
       </c>
       <c r="B91">
-        <v>6221.654120891003</v>
+        <v>3443.106736655139</v>
       </c>
       <c r="C91">
         <v>2013</v>
@@ -1547,11 +1547,11 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>2013-FSZZ024</t>
+          <t>2013-FSZZ031</t>
         </is>
       </c>
       <c r="B92">
-        <v>2194.10346155326</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C92">
         <v>2013</v>
@@ -1560,11 +1560,11 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>2013-FSZZ027</t>
+          <t>2013-FSZZ033</t>
         </is>
       </c>
       <c r="B93">
-        <v>2563.112365855231</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C93">
         <v>2013</v>
@@ -1573,11 +1573,11 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>2013-FSZZ028</t>
+          <t>2013-FSZZ034</t>
         </is>
       </c>
       <c r="B94">
-        <v>2563.112365855231</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C94">
         <v>2013</v>
@@ -1586,11 +1586,11 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>2013-FSZZ029</t>
+          <t>2013-FSZZ042</t>
         </is>
       </c>
       <c r="B95">
-        <v>4997.357801878909</v>
+        <v>6969.405211350535</v>
       </c>
       <c r="C95">
         <v>2013</v>
@@ -1599,11 +1599,11 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>2013-FSZZ030</t>
+          <t>2013-FSZZ064</t>
         </is>
       </c>
       <c r="B96">
-        <v>3443.106736655139</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C96">
         <v>2013</v>
@@ -1612,11 +1612,11 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>2013-FSZZ031</t>
+          <t>2013-FSZZ066</t>
         </is>
       </c>
       <c r="B97">
-        <v>4295.235732762522</v>
+        <v>4417.651978144046</v>
       </c>
       <c r="C97">
         <v>2013</v>
@@ -1625,76 +1625,76 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>2013-FSZZ033</t>
+          <t>2014-FSZZ009</t>
         </is>
       </c>
       <c r="B98">
-        <v>3188.160127722571</v>
+        <v>5601.384918035896</v>
       </c>
       <c r="C98">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>2013-FSZZ034</t>
+          <t>2014-FSZZ016</t>
         </is>
       </c>
       <c r="B99">
-        <v>3188.160127722571</v>
+        <v>3999.901123777936</v>
       </c>
       <c r="C99">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>2013-FSZZ042</t>
+          <t>2014-FSZZ018</t>
         </is>
       </c>
       <c r="B100">
-        <v>6969.405211350535</v>
+        <v>3999.901123777936</v>
       </c>
       <c r="C100">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>2013-FSZZ064</t>
+          <t>2014-FSZZ019</t>
         </is>
       </c>
       <c r="B101">
-        <v>2194.10346155326</v>
+        <v>3916.276930963897</v>
       </c>
       <c r="C101">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>2013-FSZZ066</t>
+          <t>2014-FSZZ020</t>
         </is>
       </c>
       <c r="B102">
-        <v>4417.651978144046</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C102">
-        <v>2013</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>2014-FSZZ009</t>
+          <t>2014-FSZZ023</t>
         </is>
       </c>
       <c r="B103">
-        <v>5601.384918035896</v>
+        <v>6840.141080416397</v>
       </c>
       <c r="C103">
         <v>2014</v>
@@ -1703,11 +1703,11 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>2014-FSZZ016</t>
+          <t>2014-FSZZ024</t>
         </is>
       </c>
       <c r="B104">
-        <v>3999.901123777936</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C104">
         <v>2014</v>
@@ -1716,11 +1716,11 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>2014-FSZZ018</t>
+          <t>2014-FSZZ027</t>
         </is>
       </c>
       <c r="B105">
-        <v>3999.901123777936</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C105">
         <v>2014</v>
@@ -1729,11 +1729,11 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>2014-FSZZ019</t>
+          <t>2014-FSZZ028</t>
         </is>
       </c>
       <c r="B106">
-        <v>3916.276930963897</v>
+        <v>2563.112365855231</v>
       </c>
       <c r="C106">
         <v>2014</v>
@@ -1742,11 +1742,11 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>2014-FSZZ020</t>
+          <t>2014-FSZZ029</t>
         </is>
       </c>
       <c r="B107">
-        <v>4974.737983049961</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C107">
         <v>2014</v>
@@ -1755,11 +1755,11 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>2014-FSZZ023</t>
+          <t>2014-FSZZ030</t>
         </is>
       </c>
       <c r="B108">
-        <v>6840.141080416397</v>
+        <v>6146.299699819397</v>
       </c>
       <c r="C108">
         <v>2014</v>
@@ -1768,11 +1768,11 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>2014-FSZZ024</t>
+          <t>2014-FSZZ031</t>
         </is>
       </c>
       <c r="B109">
-        <v>2194.10346155326</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C109">
         <v>2014</v>
@@ -1781,11 +1781,11 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>2014-FSZZ027</t>
+          <t>2014-FSZZ032</t>
         </is>
       </c>
       <c r="B110">
-        <v>2563.112365855231</v>
+        <v>4974.737983049961</v>
       </c>
       <c r="C110">
         <v>2014</v>
@@ -1794,11 +1794,11 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>2014-FSZZ028</t>
+          <t>2014-FSZZ033</t>
         </is>
       </c>
       <c r="B111">
-        <v>2563.112365855231</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C111">
         <v>2014</v>
@@ -1807,11 +1807,11 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>2014-FSZZ029</t>
+          <t>2014-FSZZ035</t>
         </is>
       </c>
       <c r="B112">
-        <v>4997.357801878909</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C112">
         <v>2014</v>
@@ -1820,11 +1820,11 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>2014-FSZZ030</t>
+          <t>2014-FSZZ037</t>
         </is>
       </c>
       <c r="B113">
-        <v>6146.299699819397</v>
+        <v>4418.34776811423</v>
       </c>
       <c r="C113">
         <v>2014</v>
@@ -1833,11 +1833,11 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>2014-FSZZ031</t>
+          <t>2014-FSZZ040</t>
         </is>
       </c>
       <c r="B114">
-        <v>1891.979915326799</v>
+        <v>3916.276930963897</v>
       </c>
       <c r="C114">
         <v>2014</v>
@@ -1846,11 +1846,11 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>2014-FSZZ032</t>
+          <t>2014-FSZZ042</t>
         </is>
       </c>
       <c r="B115">
-        <v>4974.737983049961</v>
+        <v>6969.405211350535</v>
       </c>
       <c r="C115">
         <v>2014</v>
@@ -1859,11 +1859,11 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>2014-FSZZ033</t>
+          <t>2014-FSZZ062</t>
         </is>
       </c>
       <c r="B116">
-        <v>4295.235732762522</v>
+        <v>4584.923118221286</v>
       </c>
       <c r="C116">
         <v>2014</v>
@@ -1872,11 +1872,11 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>2014-FSZZ035</t>
+          <t>2014-FSZZ064</t>
         </is>
       </c>
       <c r="B117">
-        <v>1891.979915326799</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C117">
         <v>2014</v>
@@ -1885,11 +1885,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>2014-FSZZ037</t>
+          <t>2014-FSZZ066</t>
         </is>
       </c>
       <c r="B118">
-        <v>4418.34776811423</v>
+        <v>5601.384918035896</v>
       </c>
       <c r="C118">
         <v>2014</v>
@@ -1898,11 +1898,11 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>2014-FSZZ040</t>
+          <t>2014-FSZZ080</t>
         </is>
       </c>
       <c r="B119">
-        <v>3916.276930963897</v>
+        <v>3374.303187326237</v>
       </c>
       <c r="C119">
         <v>2014</v>
@@ -1911,11 +1911,11 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>2014-FSZZ042</t>
+          <t>2014-FSZZ090</t>
         </is>
       </c>
       <c r="B120">
-        <v>6969.405211350535</v>
+        <v>3374.303187326237</v>
       </c>
       <c r="C120">
         <v>2014</v>
@@ -1924,76 +1924,76 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>2014-FSZZ062</t>
+          <t>2015-FSZZ009</t>
         </is>
       </c>
       <c r="B121">
-        <v>4584.923118221286</v>
+        <v>5601.384918035896</v>
       </c>
       <c r="C121">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>2014-FSZZ064</t>
+          <t>2015-FSZZ013</t>
         </is>
       </c>
       <c r="B122">
-        <v>2194.10346155326</v>
+        <v>2021.19222242715</v>
       </c>
       <c r="C122">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>2014-FSZZ066</t>
+          <t>2015-FSZZ014</t>
         </is>
       </c>
       <c r="B123">
-        <v>5601.384918035896</v>
+        <v>5838.504688702408</v>
       </c>
       <c r="C123">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>2014-FSZZ080</t>
+          <t>2015-FSZZ015</t>
         </is>
       </c>
       <c r="B124">
-        <v>3374.303187326237</v>
+        <v>3476.736975958923</v>
       </c>
       <c r="C124">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>2014-FSZZ090</t>
+          <t>2015-FSZZ016</t>
         </is>
       </c>
       <c r="B125">
-        <v>3374.303187326237</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C125">
-        <v>2014</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>2015-FSZZ009</t>
+          <t>2015-FSZZ018</t>
         </is>
       </c>
       <c r="B126">
-        <v>5601.384918035896</v>
+        <v>3999.901123777936</v>
       </c>
       <c r="C126">
         <v>2015</v>
@@ -2002,11 +2002,11 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>2015-FSZZ013</t>
+          <t>2015-FSZZ019</t>
         </is>
       </c>
       <c r="B127">
-        <v>2021.19222242715</v>
+        <v>5087.597664910228</v>
       </c>
       <c r="C127">
         <v>2015</v>
@@ -2015,11 +2015,11 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>2015-FSZZ014</t>
+          <t>2015-FSZZ020</t>
         </is>
       </c>
       <c r="B128">
-        <v>5838.991865039718</v>
+        <v>6221.830679149023</v>
       </c>
       <c r="C128">
         <v>2015</v>
@@ -2028,11 +2028,11 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>2015-FSZZ015</t>
+          <t>2015-FSZZ023</t>
         </is>
       </c>
       <c r="B129">
-        <v>3476.736975958923</v>
+        <v>2409.661387000257</v>
       </c>
       <c r="C129">
         <v>2015</v>
@@ -2041,11 +2041,11 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>2015-FSZZ016</t>
+          <t>2015-FSZZ024</t>
         </is>
       </c>
       <c r="B130">
-        <v>2790.894121961634</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C130">
         <v>2015</v>
@@ -2054,11 +2054,11 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>2015-FSZZ018</t>
+          <t>2015-FSZZ025</t>
         </is>
       </c>
       <c r="B131">
-        <v>3999.901123777936</v>
+        <v>1298.20838080795</v>
       </c>
       <c r="C131">
         <v>2015</v>
@@ -2067,11 +2067,11 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>2015-FSZZ019</t>
+          <t>2015-FSZZ026</t>
         </is>
       </c>
       <c r="B132">
-        <v>5087.597664910228</v>
+        <v>1298.20838080795</v>
       </c>
       <c r="C132">
         <v>2015</v>
@@ -2080,11 +2080,11 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>2015-FSZZ020</t>
+          <t>2015-FSZZ028</t>
         </is>
       </c>
       <c r="B133">
-        <v>6221.654120891003</v>
+        <v>2815.245637595413</v>
       </c>
       <c r="C133">
         <v>2015</v>
@@ -2093,11 +2093,11 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>2015-FSZZ023</t>
+          <t>2015-FSZZ029</t>
         </is>
       </c>
       <c r="B134">
-        <v>2409.661387000257</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C134">
         <v>2015</v>
@@ -2106,11 +2106,11 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>2015-FSZZ024</t>
+          <t>2015-FSZZ030</t>
         </is>
       </c>
       <c r="B135">
-        <v>2194.10346155326</v>
+        <v>6146.299699819397</v>
       </c>
       <c r="C135">
         <v>2015</v>
@@ -2119,11 +2119,11 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>2015-FSZZ025</t>
+          <t>2015-FSZZ031</t>
         </is>
       </c>
       <c r="B136">
-        <v>1298.20838080795</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C136">
         <v>2015</v>
@@ -2132,11 +2132,11 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>2015-FSZZ026</t>
+          <t>2015-FSZZ033</t>
         </is>
       </c>
       <c r="B137">
-        <v>1298.20838080795</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C137">
         <v>2015</v>
@@ -2145,11 +2145,11 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>2015-FSZZ028</t>
+          <t>2015-FSZZ034</t>
         </is>
       </c>
       <c r="B138">
-        <v>2815.245637595413</v>
+        <v>3188.781585496254</v>
       </c>
       <c r="C138">
         <v>2015</v>
@@ -2158,11 +2158,11 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>2015-FSZZ029</t>
+          <t>2015-FSZZ035</t>
         </is>
       </c>
       <c r="B139">
-        <v>4997.357801878909</v>
+        <v>1891.979915326799</v>
       </c>
       <c r="C139">
         <v>2015</v>
@@ -2171,11 +2171,11 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>2015-FSZZ030</t>
+          <t>2015-FSZZ036</t>
         </is>
       </c>
       <c r="B140">
-        <v>6146.299699819397</v>
+        <v>7089.451671321273</v>
       </c>
       <c r="C140">
         <v>2015</v>
@@ -2184,11 +2184,11 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>2015-FSZZ031</t>
+          <t>2015-FSZZ037</t>
         </is>
       </c>
       <c r="B141">
-        <v>1891.979915326799</v>
+        <v>4418.34776811423</v>
       </c>
       <c r="C141">
         <v>2015</v>
@@ -2197,11 +2197,11 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>2015-FSZZ033</t>
+          <t>2015-FSZZ042</t>
         </is>
       </c>
       <c r="B142">
-        <v>3188.160127722571</v>
+        <v>7255.277320681822</v>
       </c>
       <c r="C142">
         <v>2015</v>
@@ -2210,11 +2210,11 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>2015-FSZZ034</t>
+          <t>2015-FSZZ062</t>
         </is>
       </c>
       <c r="B143">
-        <v>3188.160127722571</v>
+        <v>4584.923118221286</v>
       </c>
       <c r="C143">
         <v>2015</v>
@@ -2223,11 +2223,11 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>2015-FSZZ035</t>
+          <t>2015-FSZZ064</t>
         </is>
       </c>
       <c r="B144">
-        <v>1891.979915326799</v>
+        <v>2194.10346155326</v>
       </c>
       <c r="C144">
         <v>2015</v>
@@ -2236,11 +2236,11 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>2015-FSZZ036</t>
+          <t>2015-FSZZ065</t>
         </is>
       </c>
       <c r="B145">
-        <v>7089.451671321273</v>
+        <v>16145.60355019285</v>
       </c>
       <c r="C145">
         <v>2015</v>
@@ -2249,11 +2249,11 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>2015-FSZZ037</t>
+          <t>2015-FSZZ066</t>
         </is>
       </c>
       <c r="B146">
-        <v>4418.34776811423</v>
+        <v>5286.748149855448</v>
       </c>
       <c r="C146">
         <v>2015</v>
@@ -2262,11 +2262,11 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>2015-FSZZ042</t>
+          <t>2015-FSZZ080</t>
         </is>
       </c>
       <c r="B147">
-        <v>7255.277320681822</v>
+        <v>3314.697572931805</v>
       </c>
       <c r="C147">
         <v>2015</v>
@@ -2275,11 +2275,11 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>2015-FSZZ062</t>
+          <t>2015-FSZZ090</t>
         </is>
       </c>
       <c r="B148">
-        <v>4584.923118221286</v>
+        <v>2021.19222242715</v>
       </c>
       <c r="C148">
         <v>2015</v>
@@ -2288,11 +2288,11 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>2015-FSZZ064</t>
+          <t>2015-FSZZ096</t>
         </is>
       </c>
       <c r="B149">
-        <v>2194.10346155326</v>
+        <v>2409.661387000257</v>
       </c>
       <c r="C149">
         <v>2015</v>
@@ -2301,102 +2301,102 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>2015-FSZZ065</t>
+          <t>2016-FSZZ020</t>
         </is>
       </c>
       <c r="B150">
-        <v>16145.93289345648</v>
+        <v>8667.09714956513</v>
       </c>
       <c r="C150">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>2015-FSZZ066</t>
+          <t>2016-FSZZ033</t>
         </is>
       </c>
       <c r="B151">
-        <v>5286.748149855448</v>
+        <v>8667.09714956513</v>
       </c>
       <c r="C151">
-        <v>2015</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>2015-FSZZ080</t>
+          <t>2017-FSZZ009</t>
         </is>
       </c>
       <c r="B152">
-        <v>3314.697572931805</v>
+        <v>3335.998351318538</v>
       </c>
       <c r="C152">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>2015-FSZZ090</t>
+          <t>2017-FSZZ010</t>
         </is>
       </c>
       <c r="B153">
-        <v>2021.19222242715</v>
+        <v>12687.65652120201</v>
       </c>
       <c r="C153">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>2015-FSZZ096</t>
+          <t>2017-FSZZ014</t>
         </is>
       </c>
       <c r="B154">
-        <v>2409.661387000257</v>
+        <v>8826.284212509814</v>
       </c>
       <c r="C154">
-        <v>2015</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>2016-FSZZ020</t>
+          <t>2017-FSZZ016</t>
         </is>
       </c>
       <c r="B155">
-        <v>8667.09714956513</v>
+        <v>5209.680412462937</v>
       </c>
       <c r="C155">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>2016-FSZZ033</t>
+          <t>2017-FSZZ019</t>
         </is>
       </c>
       <c r="B156">
-        <v>8667.09714956513</v>
+        <v>8148.70848662535</v>
       </c>
       <c r="C156">
-        <v>2016</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>2017-FSZZ009</t>
+          <t>2017-FSZZ020</t>
         </is>
       </c>
       <c r="B157">
-        <v>3326.486584972199</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C157">
         <v>2017</v>
@@ -2405,11 +2405,11 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>2017-FSZZ010</t>
+          <t>2017-FSZZ024</t>
         </is>
       </c>
       <c r="B158">
-        <v>12687.65652120201</v>
+        <v>8152.76425514684</v>
       </c>
       <c r="C158">
         <v>2017</v>
@@ -2418,11 +2418,11 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>2017-FSZZ014</t>
+          <t>2017-FSZZ027</t>
         </is>
       </c>
       <c r="B159">
-        <v>8826.570115282606</v>
+        <v>6969.405211350535</v>
       </c>
       <c r="C159">
         <v>2017</v>
@@ -2431,11 +2431,11 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>2017-FSZZ016</t>
+          <t>2017-FSZZ029</t>
         </is>
       </c>
       <c r="B160">
-        <v>5209.680412462937</v>
+        <v>4997.357801878909</v>
       </c>
       <c r="C160">
         <v>2017</v>
@@ -2444,11 +2444,11 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>2017-FSZZ019</t>
+          <t>2017-FSZZ030</t>
         </is>
       </c>
       <c r="B161">
-        <v>8148.70848662535</v>
+        <v>6146.299699819397</v>
       </c>
       <c r="C161">
         <v>2017</v>
@@ -2457,11 +2457,11 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>2017-FSZZ020</t>
+          <t>2017-FSZZ031</t>
         </is>
       </c>
       <c r="B162">
-        <v>8152.76425514684</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C162">
         <v>2017</v>
@@ -2470,11 +2470,11 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>2017-FSZZ024</t>
+          <t>2017-FSZZ033</t>
         </is>
       </c>
       <c r="B163">
-        <v>8152.76425514684</v>
+        <v>4295.235732762522</v>
       </c>
       <c r="C163">
         <v>2017</v>
@@ -2483,11 +2483,11 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>2017-FSZZ027</t>
+          <t>2017-FSZZ037</t>
         </is>
       </c>
       <c r="B164">
-        <v>6969.405211350535</v>
+        <v>6290.817514441187</v>
       </c>
       <c r="C164">
         <v>2017</v>
@@ -2496,11 +2496,11 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>2017-FSZZ029</t>
+          <t>2017-FSZZ042</t>
         </is>
       </c>
       <c r="B165">
-        <v>4997.357801878909</v>
+        <v>6969.405211350535</v>
       </c>
       <c r="C165">
         <v>2017</v>
@@ -2509,11 +2509,11 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>2017-FSZZ030</t>
+          <t>2017-FSZZ080</t>
         </is>
       </c>
       <c r="B166">
-        <v>6146.299699819397</v>
+        <v>5209.680412462937</v>
       </c>
       <c r="C166">
         <v>2017</v>
@@ -2522,11 +2522,11 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>2017-FSZZ031</t>
+          <t>2017-FSZZ106</t>
         </is>
       </c>
       <c r="B167">
-        <v>4295.235732762522</v>
+        <v>3335.998351318538</v>
       </c>
       <c r="C167">
         <v>2017</v>
@@ -2535,66 +2535,248 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>2017-FSZZ033</t>
+          <t>2018-FSZZ009</t>
         </is>
       </c>
       <c r="B168">
-        <v>4295.235732762522</v>
+        <v>2879.345238070628</v>
       </c>
       <c r="C168">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>2017-FSZZ037</t>
+          <t>2018-FSZZ010</t>
         </is>
       </c>
       <c r="B169">
-        <v>6290.817514441187</v>
+        <v>12687.65652120201</v>
       </c>
       <c r="C169">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>2017-FSZZ042</t>
+          <t>2018-FSZZ013</t>
         </is>
       </c>
       <c r="B170">
-        <v>6969.405211350535</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C170">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>2017-FSZZ080</t>
+          <t>2018-FSZZ014</t>
         </is>
       </c>
       <c r="B171">
-        <v>5209.680412462937</v>
+        <v>7564.3324226266</v>
       </c>
       <c r="C171">
-        <v>2017</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>2017-FSZZ106</t>
+          <t>2018-FSZZ016</t>
         </is>
       </c>
       <c r="B172">
-        <v>3326.486584972199</v>
+        <v>2790.894121961634</v>
       </c>
       <c r="C172">
-        <v>2017</v>
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>2018-FSZZ018</t>
+        </is>
+      </c>
+      <c r="B173">
+        <v>3999.901123777936</v>
+      </c>
+      <c r="C173">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>2018-FSZZ019</t>
+        </is>
+      </c>
+      <c r="B174">
+        <v>6396.034474578761</v>
+      </c>
+      <c r="C174">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>2018-FSZZ023</t>
+        </is>
+      </c>
+      <c r="B175">
+        <v>6840.141080416397</v>
+      </c>
+      <c r="C175">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>2018-FSZZ024</t>
+        </is>
+      </c>
+      <c r="B176">
+        <v>5734.508261394346</v>
+      </c>
+      <c r="C176">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>2018-FSZZ027</t>
+        </is>
+      </c>
+      <c r="B177">
+        <v>6969.405211350535</v>
+      </c>
+      <c r="C177">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>2018-FSZZ030</t>
+        </is>
+      </c>
+      <c r="B178">
+        <v>4788.253230563313</v>
+      </c>
+      <c r="C178">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>2018-FSZZ031</t>
+        </is>
+      </c>
+      <c r="B179">
+        <v>1891.979915326799</v>
+      </c>
+      <c r="C179">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>2018-FSZZ035</t>
+        </is>
+      </c>
+      <c r="B180">
+        <v>1891.979915326799</v>
+      </c>
+      <c r="C180">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>2018-FSZZ037</t>
+        </is>
+      </c>
+      <c r="B181">
+        <v>4418.34776811423</v>
+      </c>
+      <c r="C181">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>2018-FSZZ042</t>
+        </is>
+      </c>
+      <c r="B182">
+        <v>6969.405211350535</v>
+      </c>
+      <c r="C182">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>2018-FSZZ066</t>
+        </is>
+      </c>
+      <c r="B183">
+        <v>5601.384918035896</v>
+      </c>
+      <c r="C183">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>2018-FSZZ080</t>
+        </is>
+      </c>
+      <c r="B184">
+        <v>3314.697572931805</v>
+      </c>
+      <c r="C184">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>2018-FSZZ102</t>
+        </is>
+      </c>
+      <c r="B185">
+        <v>2879.345238070628</v>
+      </c>
+      <c r="C185">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>2018-FSZZ106</t>
+        </is>
+      </c>
+      <c r="B186">
+        <v>2988.243631299162</v>
+      </c>
+      <c r="C186">
+        <v>2018</v>
       </c>
     </row>
   </sheetData>

</xml_diff>